<commit_message>
atualizei a tabela de clipes
</commit_message>
<xml_diff>
--- a/Projeto de BC (Exemplo de dados) - fase 2.xlsx
+++ b/Projeto de BC (Exemplo de dados) - fase 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gvmail-my.sharepoint.com/personal/b51064_fgv_edu_br/Documents/2º Período/Banco de Dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silla\Downloads\BD\A2.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="710" documentId="11_AD4D361C20488DEA4E38A0E714DA708E5BDEDD97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08A2DC1C-EDB5-4348-9282-FD4FD10938DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AB6D46-6777-498C-B69C-956762FFCA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuário" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="134">
   <si>
     <t>IdUsuario</t>
   </si>
@@ -459,7 +459,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     <numFmt numFmtId="166" formatCode="#\ &quot;meses&quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +471,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -497,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -517,6 +532,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -626,9 +643,9 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FDF9B448-6E95-48EE-A75B-128966779AA1}" name="Clipe" displayName="Clipe" ref="A1:G7" totalsRowShown="0">
-  <autoFilter ref="A1:G7" xr:uid="{FDF9B448-6E95-48EE-A75B-128966779AA1}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FDF9B448-6E95-48EE-A75B-128966779AA1}" name="Clipe" displayName="Clipe" ref="A1:H7" totalsRowShown="0">
+  <autoFilter ref="A1:H7" xr:uid="{FDF9B448-6E95-48EE-A75B-128966779AA1}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F7A15F14-2976-480B-BACB-3CDBCE72A59A}" name="IdClipe"/>
     <tableColumn id="2" xr3:uid="{6FAFB718-D3DA-4259-9D59-B8F545EEB5C9}" name="TituloClipe"/>
     <tableColumn id="3" xr3:uid="{7607B58D-BE4B-48AA-82F3-74E3B528DAF2}" name="LinkClipe" dataCellStyle="Hiperlink"/>
@@ -636,6 +653,7 @@
     <tableColumn id="5" xr3:uid="{9D85891B-B612-47B2-949A-0E5E1AEC5605}" name="NCurtidasClipe"/>
     <tableColumn id="6" xr3:uid="{282C79B7-D53D-4980-964F-9F5CAB156D84}" name="DataClipe" dataDxfId="0"/>
     <tableColumn id="7" xr3:uid="{B6DEA3B4-8D3D-4CBB-ACFF-6388D54A69ED}" name="IdTransmissao"/>
+    <tableColumn id="8" xr3:uid="{9FE05A98-471A-45F7-BADF-DDAF96A96347}" name="IdUsuarioEspectador"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1016,15 +1034,15 @@
       <selection activeCell="D35" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1056,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1052,7 +1070,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -1066,7 +1084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1080,7 +1098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -1094,7 +1112,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1108,7 +1126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1122,7 +1140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -1136,7 +1154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -1150,7 +1168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -1164,7 +1182,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1178,7 +1196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -1192,7 +1210,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1206,7 +1224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1242,17 +1260,17 @@
       <selection activeCell="A2" sqref="A2:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1272,7 +1290,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1292,7 +1310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1312,7 +1330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1332,7 +1350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1352,7 +1370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1372,7 +1390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1392,7 +1410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1412,7 +1430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1442,25 +1460,24 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC094145-03D4-4094-A623-D1E74161F4EA}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="72.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>116</v>
       </c>
       <c r="B1" t="s">
@@ -1481,8 +1498,11 @@
       <c r="G1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1504,8 +1524,11 @@
       <c r="G2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1527,8 +1550,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1550,8 +1576,11 @@
       <c r="G4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1573,8 +1602,11 @@
       <c r="G5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1596,8 +1628,11 @@
       <c r="G6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1617,6 +1652,9 @@
         <v>45209.74664351852</v>
       </c>
       <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
     </row>
@@ -1644,15 +1682,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1704,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>3</v>
       </c>
@@ -1680,7 +1718,7 @@
         <v>3747040</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>4</v>
       </c>
@@ -1694,7 +1732,7 @@
         <v>4000076</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>8</v>
       </c>
@@ -1708,7 +1746,7 @@
         <v>649756</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>9</v>
       </c>
@@ -1722,7 +1760,7 @@
         <v>2405668</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>11</v>
       </c>
@@ -1736,7 +1774,7 @@
         <v>292080</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>12</v>
       </c>
@@ -1766,16 +1804,16 @@
       <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1792,7 +1830,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1809,7 +1847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1826,7 +1864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1843,7 +1881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1860,7 +1898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1877,7 +1915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1910,16 +1948,16 @@
       <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -1936,7 +1974,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>11</v>
       </c>
@@ -1953,7 +1991,7 @@
         <v>45069.597337962965</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -1970,7 +2008,7 @@
         <v>44446.948553240742</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1987,7 +2025,7 @@
         <v>44208.479456018518</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>9</v>
       </c>
@@ -2004,7 +2042,7 @@
         <v>43951.802546296298</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2021,7 +2059,7 @@
         <v>42565.33697916667</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -2038,7 +2076,7 @@
         <v>43033.743402777778</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E8" s="4"/>
     </row>
   </sheetData>
@@ -2057,17 +2095,17 @@
       <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -2087,7 +2125,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2107,7 +2145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2127,7 +2165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2147,7 +2185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2167,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2187,7 +2225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2223,17 +2261,17 @@
       <selection activeCell="A2" sqref="A2:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2256,7 +2294,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2279,7 +2317,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2302,7 +2340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2325,7 +2363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2348,7 +2386,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2371,7 +2409,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2410,13 +2448,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -2424,7 +2462,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2432,7 +2470,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2440,7 +2478,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2448,7 +2486,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2456,7 +2494,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2464,7 +2502,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2472,7 +2510,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2496,13 +2534,13 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2510,7 +2548,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2518,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2526,7 +2564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2534,7 +2572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2542,7 +2580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2550,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2558,7 +2596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2566,7 +2604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2590,14 +2628,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2608,7 +2646,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2619,7 +2657,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2630,7 +2668,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2641,7 +2679,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2652,7 +2690,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2663,7 +2701,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>